<commit_message>
add: gas cell functions test.
</commit_message>
<xml_diff>
--- a/data/spreadsheet.xlsx
+++ b/data/spreadsheet.xlsx
@@ -52,6 +52,13 @@
     <t>name</t>
   </si>
   <si>
+    <t>christmas</t>
+  </si>
+  <si>
+    <t>happy
+new year</t>
+  </si>
+  <si>
     <t>taro</t>
   </si>
   <si>
@@ -59,13 +66,6 @@
   </si>
   <si>
     <t>saburo</t>
-  </si>
-  <si>
-    <t>christmas</t>
-  </si>
-  <si>
-    <t>happy
-new year</t>
   </si>
 </sst>
 </file>
@@ -101,10 +101,10 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -118,20 +118,20 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2143125" cy="2133600"/>
+    <xdr:ext cx="2152650" cy="2143125"/>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Shape 3"/>
+        <xdr:cNvPr id="4" name="Shape 4"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="876650" y="711075"/>
-          <a:ext cx="2123400" cy="2113800"/>
+          <a:off x="4274438" y="2713200"/>
+          <a:ext cx="2143125" cy="2133600"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -162,6 +162,8 @@
             <a:spcAft>
               <a:spcPts val="0"/>
             </a:spcAft>
+            <a:buSzPts val="1400"/>
+            <a:buFont typeface="Arial"/>
             <a:buNone/>
           </a:pPr>
           <a:r>
@@ -185,20 +187,20 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:colOff>123825</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3800475" cy="2981325"/>
+    <xdr:ext cx="3810000" cy="2990850"/>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Shape 5"/>
+        <xdr:cNvPr id="3" name="Shape 3"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3450525" y="2294100"/>
-          <a:ext cx="3790950" cy="2971800"/>
+          <a:off x="3445763" y="2289338"/>
+          <a:ext cx="3800475" cy="2981325"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -467,7 +469,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
@@ -475,7 +477,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1"/>
@@ -1523,7 +1525,7 @@
       <c r="C2" s="1">
         <v>1.0</v>
       </c>
-      <c r="D2" s="1" t="str">
+      <c r="D2" s="2" t="str">
         <f t="array" ref="D2">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -1542,7 +1544,7 @@
       <c r="E2" s="1">
         <v>1.0</v>
       </c>
-      <c r="F2" s="1" t="str">
+      <c r="F2" s="2" t="str">
         <f t="array" ref="F2">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -1563,7 +1565,7 @@
       <c r="C3" s="1">
         <v>2.0</v>
       </c>
-      <c r="D3" s="1" t="str">
+      <c r="D3" s="2" t="str">
         <f t="array" ref="D3">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -1583,7 +1585,7 @@
       <c r="E3" s="1">
         <v>3.0</v>
       </c>
-      <c r="F3" s="1" t="str">
+      <c r="F3" s="2" t="str">
         <f t="array" ref="F3">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -1601,7 +1603,7 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="D4" s="1" t="str">
+      <c r="D4" s="2" t="str">
         <f t="array" ref="D4">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -1620,7 +1622,7 @@
       <c r="E4" s="1">
         <v>2.0</v>
       </c>
-      <c r="F4" s="1" t="str">
+      <c r="F4" s="2" t="str">
         <f t="array" ref="F4">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -1638,7 +1640,7 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="D5" s="1" t="str">
+      <c r="D5" s="2" t="str">
         <f t="array" ref="D5">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -1654,7 +1656,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F5" s="1" t="str">
+      <c r="F5" s="2" t="str">
         <f t="array" ref="F5">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -1672,7 +1674,7 @@
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="D6" s="1" t="str">
+      <c r="D6" s="2" t="str">
         <f t="array" ref="D6">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -1688,7 +1690,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F6" s="1" t="str">
+      <c r="F6" s="2" t="str">
         <f t="array" ref="F6">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -1706,7 +1708,7 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="D7" s="1" t="str">
+      <c r="D7" s="2" t="str">
         <f t="array" ref="D7">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -1722,7 +1724,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F7" s="1" t="str">
+      <c r="F7" s="2" t="str">
         <f t="array" ref="F7">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -1740,7 +1742,7 @@
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="D8" s="1" t="str">
+      <c r="D8" s="2" t="str">
         <f t="array" ref="D8">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -1756,7 +1758,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F8" s="1" t="str">
+      <c r="F8" s="2" t="str">
         <f t="array" ref="F8">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -1774,7 +1776,7 @@
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="D9" s="1" t="str">
+      <c r="D9" s="2" t="str">
         <f t="array" ref="D9">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -1790,7 +1792,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F9" s="1" t="str">
+      <c r="F9" s="2" t="str">
         <f t="array" ref="F9">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -1808,7 +1810,7 @@
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="F10" s="1" t="str">
+      <c r="F10" s="2" t="str">
         <f t="array" ref="F10">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -1829,7 +1831,7 @@
       <c r="C11" s="1">
         <v>1.0</v>
       </c>
-      <c r="D11" s="1" t="str">
+      <c r="D11" s="2" t="str">
         <f t="shared" ref="D11:D19" si="1">GetCellFilterByColumnValue(
   "events!1:1!id," &amp; GetCellByColumnName("1:1," &amp; ROW(11:11) &amp; ",event_id") &amp;",name"
 )</f>
@@ -1838,7 +1840,7 @@
       <c r="E11" s="1">
         <v>1.0</v>
       </c>
-      <c r="F11" s="1" t="str">
+      <c r="F11" s="2" t="str">
         <f t="shared" ref="F11:F19" si="2">GetCellFilterByColumnValue(
   "users!1:1!id," &amp; GetCellByColumnName("1:1," &amp; ROW(11:11) &amp; ",user_id") &amp;",name"
 )</f>
@@ -1849,7 +1851,7 @@
       <c r="C12" s="1">
         <v>2.0</v>
       </c>
-      <c r="D12" s="1" t="str">
+      <c r="D12" s="2" t="str">
         <f t="shared" si="1"/>
         <v>happy
 new year</v>
@@ -1857,20 +1859,20 @@
       <c r="E12" s="1">
         <v>2.0</v>
       </c>
-      <c r="F12" s="1" t="str">
+      <c r="F12" s="2" t="str">
         <f t="shared" si="2"/>
         <v>jiro</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="D13" s="1" t="str">
+      <c r="D13" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E13" s="1">
         <v>3.0</v>
       </c>
-      <c r="F13" s="1" t="str">
+      <c r="F13" s="2" t="str">
         <f t="shared" si="2"/>
         <v>saburo</v>
       </c>
@@ -1879,61 +1881,61 @@
       <c r="B14" s="1">
         <v>5.0</v>
       </c>
-      <c r="D14" s="1" t="str">
+      <c r="D14" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F14" s="1" t="str">
+      <c r="F14" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="D15" s="1" t="str">
+      <c r="D15" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F15" s="1" t="str">
+      <c r="F15" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="D16" s="1" t="str">
+      <c r="D16" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F16" s="1" t="str">
+      <c r="F16" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="D17" s="1" t="str">
+      <c r="D17" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F17" s="1" t="str">
+      <c r="F17" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="D18" s="1" t="str">
+      <c r="D18" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F18" s="1" t="str">
+      <c r="F18" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="D19" s="1" t="str">
+      <c r="D19" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F19" s="1" t="str">
+      <c r="F19" s="2" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2950,7 +2952,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
@@ -2958,7 +2960,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
@@ -2966,12 +2968,12 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1"/>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="C6" s="2"/>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" ht="15.75" customHeight="1"/>
     <row r="8" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
fix:  csv and yaml column lenght when dump.
</commit_message>
<xml_diff>
--- a/data/spreadsheet.xlsx
+++ b/data/spreadsheet.xlsx
@@ -13,47 +13,31 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="C6">
-      <text>
-        <t xml:space="preserve">aaaaaaaaa
-</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+  <si>
+    <t>スプレットシートマスター</t>
+  </si>
   <si>
     <t>id</t>
   </si>
   <si>
+    <t>name</t>
+  </si>
+  <si>
     <t>rank</t>
   </si>
   <si>
-    <t>スプレットシートマスター</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>event_id</t>
   </si>
   <si>
     <t>event_name</t>
   </si>
   <si>
+    <t>user_id</t>
+  </si>
+  <si>
     <t>christmas</t>
-  </si>
-  <si>
-    <t>user_id</t>
   </si>
   <si>
     <t>user_name</t>
@@ -189,22 +173,22 @@
     <t>brew install diff-pdf</t>
   </si>
   <si>
+    <t>npm run compare commit_hash 123456789abcd</t>
+  </si>
+  <si>
+    <t>シートの順番変えられた時とか差分いっぱい出るからしんどい</t>
+  </si>
+  <si>
+    <t>余談</t>
+  </si>
+  <si>
     <t>jiro</t>
   </si>
   <si>
-    <t>npm run compare commit_hash 123456789abcd</t>
-  </si>
-  <si>
-    <t>シートの順番変えられた時とか差分いっぱい出るからしんどい</t>
+    <t>src/gas</t>
   </si>
   <si>
     <t>saburo</t>
-  </si>
-  <si>
-    <t>余談</t>
-  </si>
-  <si>
-    <t>src/gas</t>
   </si>
   <si>
     <t>GASでのみ使用するスクリプト</t>
@@ -232,7 +216,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -242,6 +226,7 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -285,21 +270,33 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -318,11 +315,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
+      <xdr:colOff>171450</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2162175" cy="2152650"/>
+    <xdr:ext cx="2171700" cy="2162175"/>
     <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="Shape 3"/>
@@ -330,8 +327,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4269675" y="2708438"/>
-          <a:ext cx="2152650" cy="2143125"/>
+          <a:off x="4264913" y="2703675"/>
+          <a:ext cx="2162175" cy="2152650"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -383,70 +380,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="3819525" cy="3000375"/>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Shape 4"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3441000" y="2284575"/>
-          <a:ext cx="3810000" cy="2990850"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd fmla="val 16667" name="adj"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="CFE2F3"/>
-        </a:solidFill>
-        <a:ln cap="flat" cmpd="sng" w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd len="sm" w="sm" type="none"/>
-          <a:tailEnd len="sm" w="sm" type="none"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr anchorCtr="0" anchor="ctr" bIns="91425" lIns="91425" spcFirstLastPara="1" rIns="91425" wrap="square" tIns="91425">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buSzPts val="1400"/>
-            <a:buFont typeface="Arial"/>
-            <a:buNone/>
-          </a:pPr>
-          <a:r>
-            <a:t/>
-          </a:r>
-          <a:endParaRPr sz="1400"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -661,8 +595,8 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -689,366 +623,439 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
     </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
     </row>
     <row r="4">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="7"/>
     </row>
     <row r="5">
-      <c r="A5" s="1"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
     </row>
     <row r="7">
-      <c r="B7" s="1" t="s">
-        <v>13</v>
+      <c r="B7" s="7"/>
+      <c r="D7" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8">
-      <c r="C8" s="1" t="s">
-        <v>14</v>
+      <c r="C8" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9">
-      <c r="D9" s="1" t="s">
-        <v>15</v>
+      <c r="D9" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10">
-      <c r="C10" s="1"/>
+      <c r="C10" s="7"/>
+      <c r="E10" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11">
-      <c r="C11" s="1" t="s">
-        <v>16</v>
+      <c r="C11" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12">
-      <c r="D12" s="1" t="s">
-        <v>17</v>
+      <c r="D12" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13">
-      <c r="C13" s="1"/>
-      <c r="E13" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="7"/>
     </row>
     <row r="14">
-      <c r="C14" s="1"/>
+      <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="7"/>
     </row>
     <row r="15">
-      <c r="C15" s="1" t="s">
-        <v>19</v>
+      <c r="C15" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="16">
-      <c r="D16" s="1" t="s">
-        <v>20</v>
+      <c r="D16" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17">
-      <c r="D17" s="1" t="s">
-        <v>21</v>
+      <c r="D17" s="7"/>
+      <c r="E17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="E18" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="1" t="s">
-        <v>22</v>
+      <c r="B19" s="7"/>
+      <c r="E19" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="20">
-      <c r="C20" s="1" t="s">
-        <v>23</v>
+      <c r="C20" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="D21" s="1" t="s">
-        <v>24</v>
+      <c r="D21" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="E22" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="C22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="E23" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="D23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="E24" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="C24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="C25" s="1"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="C26" s="1" t="s">
-        <v>28</v>
+      <c r="C26" s="7"/>
+      <c r="D26" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="D27" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1"/>
+      <c r="C27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="D28" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="C29" s="1" t="s">
-        <v>30</v>
+      <c r="C29" s="7"/>
+      <c r="E29" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="D30" s="1" t="s">
-        <v>31</v>
+      <c r="D30" s="7"/>
+      <c r="E30" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="C31" s="1"/>
+      <c r="C31" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="C32" s="1" t="s">
-        <v>32</v>
+      <c r="C32" s="7"/>
+      <c r="D32" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="D33" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="C33" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="7"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="D34" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1"/>
+      <c r="C34" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="7"/>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="D35" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="C36" s="1" t="s">
-        <v>35</v>
+      <c r="C36" s="7"/>
+      <c r="D36" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="D37" s="1" t="s">
-        <v>36</v>
+      <c r="D37" s="7"/>
+      <c r="E37" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="E38" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="C38" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="7"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="E39" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" ht="15.75" customHeight="1"/>
+      <c r="D39" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E39" s="7"/>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="E40" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="C41" s="1" t="s">
-        <v>39</v>
+      <c r="C41" s="7"/>
+      <c r="E41" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="D42" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" ht="15.75" customHeight="1"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="D43" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="C44" s="1" t="s">
-        <v>41</v>
+      <c r="C44" s="7"/>
+      <c r="D44" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="C45" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="A45" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="7"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="C46" s="1"/>
-      <c r="D46" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="B46" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="D47" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="C47" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D47" s="7"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="E48" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="49" ht="15.75" customHeight="1"/>
+      <c r="B48" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E48" s="7"/>
+    </row>
+    <row r="49" ht="15.75" customHeight="1">
+      <c r="C49" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="C50" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="B50" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="7"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="D51" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="C51" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D51" s="7"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="D52" s="1"/>
-      <c r="E52" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="B52" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="D53" s="1"/>
-      <c r="E53" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="C53" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="D54" s="1"/>
-      <c r="E54" s="1" t="s">
+      <c r="D54" s="7"/>
+      <c r="E54" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="D55" s="1" t="s">
+      <c r="D55" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" ht="15.75" customHeight="1">
+      <c r="D56" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
-      <c r="D56" s="1" t="s">
+    <row r="57" ht="15.75" customHeight="1">
+      <c r="D57" s="7"/>
+    </row>
+    <row r="58" ht="15.75" customHeight="1">
+      <c r="A58" s="12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" ht="15.75" customHeight="1">
-      <c r="D57" s="1"/>
-    </row>
-    <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="8" t="s">
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="12"/>
+      <c r="L58" s="12"/>
+      <c r="M58" s="12"/>
+      <c r="N58" s="12"/>
+      <c r="O58" s="12"/>
+      <c r="P58" s="12"/>
+      <c r="Q58" s="12"/>
+      <c r="R58" s="12"/>
+      <c r="S58" s="12"/>
+      <c r="T58" s="12"/>
+      <c r="U58" s="12"/>
+      <c r="V58" s="12"/>
+      <c r="W58" s="12"/>
+      <c r="X58" s="12"/>
+      <c r="Y58" s="12"/>
+    </row>
+    <row r="59" ht="15.75" customHeight="1">
+      <c r="B59" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
-      <c r="H58" s="8"/>
-      <c r="I58" s="8"/>
-      <c r="J58" s="8"/>
-      <c r="K58" s="8"/>
-      <c r="L58" s="8"/>
-      <c r="M58" s="8"/>
-      <c r="N58" s="8"/>
-      <c r="O58" s="8"/>
-      <c r="P58" s="8"/>
-      <c r="Q58" s="8"/>
-      <c r="R58" s="8"/>
-      <c r="S58" s="8"/>
-      <c r="T58" s="8"/>
-      <c r="U58" s="8"/>
-      <c r="V58" s="8"/>
-      <c r="W58" s="8"/>
-      <c r="X58" s="8"/>
-      <c r="Y58" s="8"/>
-    </row>
-    <row r="59" ht="15.75" customHeight="1">
-      <c r="B59" s="1" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="7" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="7" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="7" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1"/>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="11" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="7" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="7" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="7" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2003,26 +2010,26 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1">
+      <c r="A2" s="3">
         <v>1.0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1">
+      <c r="A3" s="3">
         <v>2.0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3042,36 +3049,36 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1">
+      <c r="A2" s="3">
         <v>1.0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>1.0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>1.0</v>
       </c>
-      <c r="D2" s="6" t="str">
+      <c r="D2" s="3" t="str">
         <f t="array" ref="D2">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3087,10 +3094,10 @@
 )</f>
         <v>christmas</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="3">
         <v>1.0</v>
       </c>
-      <c r="F2" s="6" t="str">
+      <c r="F2" s="3" t="str">
         <f t="array" ref="F2">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3108,10 +3115,10 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>2.0</v>
       </c>
-      <c r="D3" s="6" t="str">
+      <c r="D3" s="3" t="str">
         <f t="array" ref="D3">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3128,10 +3135,10 @@
         <v>happy
 new year</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="3">
         <v>3.0</v>
       </c>
-      <c r="F3" s="6" t="str">
+      <c r="F3" s="3" t="str">
         <f t="array" ref="F3">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3149,7 +3156,7 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="D4" s="6" t="str">
+      <c r="D4" s="3" t="str">
         <f t="array" ref="D4">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3165,10 +3172,10 @@
 )</f>
         <v/>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="3">
         <v>2.0</v>
       </c>
-      <c r="F4" s="6" t="str">
+      <c r="F4" s="3" t="str">
         <f t="array" ref="F4">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3186,7 +3193,7 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="D5" s="6" t="str">
+      <c r="D5" s="3" t="str">
         <f t="array" ref="D5">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3202,7 +3209,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F5" s="6" t="str">
+      <c r="F5" s="3" t="str">
         <f t="array" ref="F5">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3220,7 +3227,7 @@
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="D6" s="6" t="str">
+      <c r="D6" s="3" t="str">
         <f t="array" ref="D6">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3236,7 +3243,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F6" s="6" t="str">
+      <c r="F6" s="3" t="str">
         <f t="array" ref="F6">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3254,7 +3261,7 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="D7" s="6" t="str">
+      <c r="D7" s="3" t="str">
         <f t="array" ref="D7">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3270,7 +3277,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F7" s="6" t="str">
+      <c r="F7" s="3" t="str">
         <f t="array" ref="F7">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3288,7 +3295,7 @@
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="D8" s="6" t="str">
+      <c r="D8" s="3" t="str">
         <f t="array" ref="D8">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3304,7 +3311,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F8" s="6" t="str">
+      <c r="F8" s="3" t="str">
         <f t="array" ref="F8">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3322,7 +3329,7 @@
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="D9" s="6" t="str">
+      <c r="D9" s="3" t="str">
         <f t="array" ref="D9">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3338,7 +3345,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F9" s="6" t="str">
+      <c r="F9" s="3" t="str">
         <f t="array" ref="F9">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3356,7 +3363,7 @@
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="F10" s="6" t="str">
+      <c r="F10" s="3" t="str">
         <f t="array" ref="F10">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3374,19 +3381,19 @@
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="C11" s="1">
+      <c r="C11" s="3">
         <v>1.0</v>
       </c>
-      <c r="D11" s="6" t="str">
+      <c r="D11" s="3" t="str">
         <f t="shared" ref="D11:D19" si="1">GetCellFilterByColumnValue(
   "events!1:1!id," &amp; GetCellByColumnName("1:1," &amp; ROW(11:11) &amp; ",event_id") &amp;",name"
 )</f>
         <v>christmas</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="3">
         <v>1.0</v>
       </c>
-      <c r="F11" s="6" t="str">
+      <c r="F11" s="3" t="str">
         <f t="shared" ref="F11:F19" si="2">GetCellFilterByColumnValue(
   "users!1:1!id," &amp; GetCellByColumnName("1:1," &amp; ROW(11:11) &amp; ",user_id") &amp;",name"
 )</f>
@@ -3394,94 +3401,94 @@
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="C12" s="1">
+      <c r="C12" s="3">
         <v>2.0</v>
       </c>
-      <c r="D12" s="6" t="str">
+      <c r="D12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>happy
 new year</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="3">
         <v>2.0</v>
       </c>
-      <c r="F12" s="6" t="str">
+      <c r="F12" s="3" t="str">
         <f t="shared" si="2"/>
         <v>jiro</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="D13" s="6" t="str">
+      <c r="D13" s="3" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="3">
         <v>3.0</v>
       </c>
-      <c r="F13" s="6" t="str">
+      <c r="F13" s="3" t="str">
         <f t="shared" si="2"/>
         <v>saburo</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="B14" s="1">
+      <c r="B14" s="3">
         <v>5.0</v>
       </c>
-      <c r="D14" s="6" t="str">
+      <c r="D14" s="3" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F14" s="6" t="str">
+      <c r="F14" s="3" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="D15" s="6" t="str">
+      <c r="D15" s="3" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F15" s="6" t="str">
+      <c r="F15" s="3" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="D16" s="6" t="str">
+      <c r="D16" s="3" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F16" s="6" t="str">
+      <c r="F16" s="3" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="D17" s="6" t="str">
+      <c r="D17" s="3" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F17" s="6" t="str">
+      <c r="F17" s="3" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="D18" s="6" t="str">
+      <c r="D18" s="3" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F18" s="6" t="str">
+      <c r="F18" s="3" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="D19" s="6" t="str">
+      <c r="D19" s="3" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F19" s="6" t="str">
+      <c r="F19" s="3" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4486,40 +4493,40 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1">
+      <c r="A2" s="3">
         <v>1.0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1">
+      <c r="A3" s="3">
         <v>2.0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>52</v>
+      <c r="B3" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1">
+      <c r="A4" s="3">
         <v>3.0</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>55</v>
+      <c r="B4" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1"/>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="C6" s="1"/>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1"/>
     <row r="8" ht="15.75" customHeight="1"/>
@@ -5516,7 +5523,6 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add: memo column in rankings.
</commit_message>
<xml_diff>
--- a/data/spreadsheet.xlsx
+++ b/data/spreadsheet.xlsx
@@ -14,33 +14,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>rank</t>
+  </si>
+  <si>
+    <t>event_id</t>
+  </si>
+  <si>
+    <t>event_name</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
   <si>
     <t>スプレットシートマスター</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
-    <t>rank</t>
-  </si>
-  <si>
-    <t>event_id</t>
-  </si>
-  <si>
-    <t>event_name</t>
-  </si>
-  <si>
-    <t>user_id</t>
+    <t>user_name</t>
+  </si>
+  <si>
+    <t>memo</t>
   </si>
   <si>
     <t>christmas</t>
-  </si>
-  <si>
-    <t>user_name</t>
   </si>
   <si>
     <t>happy
@@ -158,58 +161,58 @@
     <t>Gitのコミットハッシュでスプレットシートの差分をビジュアライズに比較する</t>
   </si>
   <si>
+    <t>使うときは</t>
+  </si>
+  <si>
+    <t>LibreOfficeをインストール</t>
+  </si>
+  <si>
+    <t>brew cask install xquartz</t>
+  </si>
+  <si>
+    <t>brew install diff-pdf</t>
+  </si>
+  <si>
+    <t>npm run compare commit_hash 123456789abcd</t>
+  </si>
+  <si>
+    <t>シートの順番変えられた時とか差分いっぱい出るからしんどい</t>
+  </si>
+  <si>
+    <t>余談</t>
+  </si>
+  <si>
+    <t>src/gas</t>
+  </si>
+  <si>
+    <t>GASでのみ使用するスクリプト</t>
+  </si>
+  <si>
+    <t>src/tasks</t>
+  </si>
+  <si>
+    <t>ローカルでのみ使用するスクリプト</t>
+  </si>
+  <si>
+    <t>テストについて</t>
+  </si>
+  <si>
+    <t>GASないでのみ使えるものは全部モックで検証</t>
+  </si>
+  <si>
+    <t>最近読めないExcel関数</t>
+  </si>
+  <si>
+    <t>INDEX MATCH</t>
+  </si>
+  <si>
     <t>taro</t>
   </si>
   <si>
-    <t>使うときは</t>
-  </si>
-  <si>
-    <t>LibreOfficeをインストール</t>
-  </si>
-  <si>
-    <t>brew cask install xquartz</t>
-  </si>
-  <si>
-    <t>brew install diff-pdf</t>
-  </si>
-  <si>
-    <t>npm run compare commit_hash 123456789abcd</t>
-  </si>
-  <si>
-    <t>シートの順番変えられた時とか差分いっぱい出るからしんどい</t>
-  </si>
-  <si>
-    <t>余談</t>
-  </si>
-  <si>
     <t>jiro</t>
   </si>
   <si>
-    <t>src/gas</t>
-  </si>
-  <si>
     <t>saburo</t>
-  </si>
-  <si>
-    <t>GASでのみ使用するスクリプト</t>
-  </si>
-  <si>
-    <t>src/tasks</t>
-  </si>
-  <si>
-    <t>ローカルでのみ使用するスクリプト</t>
-  </si>
-  <si>
-    <t>テストについて</t>
-  </si>
-  <si>
-    <t>GASないでのみ使えるものは全部モックで検証</t>
-  </si>
-  <si>
-    <t>最近読めないExcel関数</t>
-  </si>
-  <si>
-    <t>INDEX MATCH</t>
   </si>
 </sst>
 </file>
@@ -274,13 +277,13 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -294,10 +297,10 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -595,43 +598,43 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5"/>
       <c r="B3" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -658,22 +661,22 @@
       <c r="Y3" s="5"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>12</v>
+      <c r="A4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B4" s="7"/>
     </row>
     <row r="5">
       <c r="A5" s="7"/>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -701,181 +704,181 @@
     <row r="7">
       <c r="B7" s="7"/>
       <c r="D7" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
-      <c r="C8" s="3" t="s">
-        <v>16</v>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9">
-      <c r="D9" s="3" t="s">
-        <v>17</v>
+      <c r="D9" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="C10" s="7"/>
       <c r="E10" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
-      <c r="C11" s="3" t="s">
-        <v>19</v>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12">
-      <c r="D12" s="3" t="s">
-        <v>20</v>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13">
       <c r="C13" s="7"/>
       <c r="D13" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E13" s="7"/>
     </row>
     <row r="14">
       <c r="B14" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" s="7"/>
     </row>
     <row r="15">
-      <c r="C15" s="3" t="s">
-        <v>23</v>
+      <c r="C15" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16">
-      <c r="D16" s="3" t="s">
-        <v>24</v>
+      <c r="D16" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17">
       <c r="D17" s="7"/>
       <c r="E17" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18">
       <c r="E18" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="7"/>
       <c r="E19" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20">
-      <c r="C20" s="3" t="s">
-        <v>28</v>
+      <c r="C20" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="D21" s="3" t="s">
-        <v>29</v>
+      <c r="D21" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="C22" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E22" s="10"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="D23" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E23" s="7"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="C24" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E24" s="7"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="C25" s="7"/>
       <c r="D25" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="C26" s="7"/>
       <c r="D26" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="C27" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D27" s="7"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="D28" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="C29" s="7"/>
       <c r="E29" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="D30" s="7"/>
       <c r="E30" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="C31" s="3" t="s">
-        <v>39</v>
+      <c r="C31" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="C32" s="7"/>
       <c r="D32" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="C33" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D33" s="7"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="C34" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D34" s="7"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="D35" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="C36" s="7"/>
       <c r="D36" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="D37" s="7"/>
       <c r="E37" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="C38" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E38" s="7"/>
     </row>
@@ -921,50 +924,50 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="B46" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="C47" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D47" s="7"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="B48" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E48" s="7"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="C49" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="B50" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C50" s="7"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="C51" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D51" s="7"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="B52" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="C53" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
@@ -989,74 +992,74 @@
       <c r="D57" s="7"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="12" t="s">
+      <c r="A58" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
-      <c r="H58" s="12"/>
-      <c r="I58" s="12"/>
-      <c r="J58" s="12"/>
-      <c r="K58" s="12"/>
-      <c r="L58" s="12"/>
-      <c r="M58" s="12"/>
-      <c r="N58" s="12"/>
-      <c r="O58" s="12"/>
-      <c r="P58" s="12"/>
-      <c r="Q58" s="12"/>
-      <c r="R58" s="12"/>
-      <c r="S58" s="12"/>
-      <c r="T58" s="12"/>
-      <c r="U58" s="12"/>
-      <c r="V58" s="12"/>
-      <c r="W58" s="12"/>
-      <c r="X58" s="12"/>
-      <c r="Y58" s="12"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="11"/>
+      <c r="L58" s="11"/>
+      <c r="M58" s="11"/>
+      <c r="N58" s="11"/>
+      <c r="O58" s="11"/>
+      <c r="P58" s="11"/>
+      <c r="Q58" s="11"/>
+      <c r="R58" s="11"/>
+      <c r="S58" s="11"/>
+      <c r="T58" s="11"/>
+      <c r="U58" s="11"/>
+      <c r="V58" s="11"/>
+      <c r="W58" s="11"/>
+      <c r="X58" s="11"/>
+      <c r="Y58" s="11"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="B59" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="C60" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="B61" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="C62" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1"/>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="B64" s="11" t="s">
-        <v>61</v>
+      <c r="B64" s="12" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="C65" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1">
       <c r="B67" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="C68" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1"/>
@@ -2010,27 +2013,27 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>2</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="3">
+      <c r="A2" s="1">
         <v>1.0</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="3">
+      <c r="A3" s="1">
         <v>2.0</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1"/>
@@ -3049,36 +3052,39 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="3">
+      <c r="A2" s="1">
         <v>1.0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <v>1.0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1">
         <v>1.0</v>
       </c>
-      <c r="D2" s="3" t="str">
+      <c r="D2" s="1" t="str">
         <f t="array" ref="D2">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3094,10 +3100,10 @@
 )</f>
         <v>christmas</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="1">
         <v>1.0</v>
       </c>
-      <c r="F2" s="3" t="str">
+      <c r="F2" s="1" t="str">
         <f t="array" ref="F2">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3115,10 +3121,10 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <v>2.0</v>
       </c>
-      <c r="D3" s="3" t="str">
+      <c r="D3" s="1" t="str">
         <f t="array" ref="D3">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3135,10 +3141,10 @@
         <v>happy
 new year</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>3.0</v>
       </c>
-      <c r="F3" s="3" t="str">
+      <c r="F3" s="1" t="str">
         <f t="array" ref="F3">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3156,7 +3162,7 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="D4" s="3" t="str">
+      <c r="D4" s="1" t="str">
         <f t="array" ref="D4">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3172,10 +3178,10 @@
 )</f>
         <v/>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>2.0</v>
       </c>
-      <c r="F4" s="3" t="str">
+      <c r="F4" s="1" t="str">
         <f t="array" ref="F4">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3193,7 +3199,7 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="D5" s="3" t="str">
+      <c r="D5" s="1" t="str">
         <f t="array" ref="D5">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3209,7 +3215,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F5" s="3" t="str">
+      <c r="F5" s="1" t="str">
         <f t="array" ref="F5">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3227,7 +3233,7 @@
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="D6" s="3" t="str">
+      <c r="D6" s="1" t="str">
         <f t="array" ref="D6">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3243,7 +3249,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F6" s="3" t="str">
+      <c r="F6" s="1" t="str">
         <f t="array" ref="F6">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3261,7 +3267,7 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="D7" s="3" t="str">
+      <c r="D7" s="1" t="str">
         <f t="array" ref="D7">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3277,7 +3283,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F7" s="3" t="str">
+      <c r="F7" s="1" t="str">
         <f t="array" ref="F7">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3295,7 +3301,7 @@
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="D8" s="3" t="str">
+      <c r="D8" s="1" t="str">
         <f t="array" ref="D8">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3311,7 +3317,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F8" s="3" t="str">
+      <c r="F8" s="1" t="str">
         <f t="array" ref="F8">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3329,7 +3335,7 @@
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="D9" s="3" t="str">
+      <c r="D9" s="1" t="str">
         <f t="array" ref="D9">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3345,7 +3351,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F9" s="3" t="str">
+      <c r="F9" s="1" t="str">
         <f t="array" ref="F9">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3363,7 +3369,7 @@
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="F10" s="3" t="str">
+      <c r="F10" s="1" t="str">
         <f t="array" ref="F10">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3381,19 +3387,19 @@
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="C11" s="3">
+      <c r="C11" s="1">
         <v>1.0</v>
       </c>
-      <c r="D11" s="3" t="str">
+      <c r="D11" s="1" t="str">
         <f t="shared" ref="D11:D19" si="1">GetCellFilterByColumnValue(
   "events!1:1!id," &amp; GetCellByColumnName("1:1," &amp; ROW(11:11) &amp; ",event_id") &amp;",name"
 )</f>
         <v>christmas</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="1">
         <v>1.0</v>
       </c>
-      <c r="F11" s="3" t="str">
+      <c r="F11" s="1" t="str">
         <f t="shared" ref="F11:F19" si="2">GetCellFilterByColumnValue(
   "users!1:1!id," &amp; GetCellByColumnName("1:1," &amp; ROW(11:11) &amp; ",user_id") &amp;",name"
 )</f>
@@ -3401,94 +3407,94 @@
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="C12" s="3">
+      <c r="C12" s="1">
         <v>2.0</v>
       </c>
-      <c r="D12" s="3" t="str">
+      <c r="D12" s="1" t="str">
         <f t="shared" si="1"/>
         <v>happy
 new year</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="1">
         <v>2.0</v>
       </c>
-      <c r="F12" s="3" t="str">
+      <c r="F12" s="1" t="str">
         <f t="shared" si="2"/>
         <v>jiro</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="D13" s="3" t="str">
+      <c r="D13" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="1">
         <v>3.0</v>
       </c>
-      <c r="F13" s="3" t="str">
+      <c r="F13" s="1" t="str">
         <f t="shared" si="2"/>
         <v>saburo</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="B14" s="3">
+      <c r="B14" s="1">
         <v>5.0</v>
       </c>
-      <c r="D14" s="3" t="str">
+      <c r="D14" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F14" s="3" t="str">
+      <c r="F14" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="D15" s="3" t="str">
+      <c r="D15" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F15" s="3" t="str">
+      <c r="F15" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="D16" s="3" t="str">
+      <c r="D16" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F16" s="3" t="str">
+      <c r="F16" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="D17" s="3" t="str">
+      <c r="D17" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F17" s="3" t="str">
+      <c r="F17" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="D18" s="3" t="str">
+      <c r="D18" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F18" s="3" t="str">
+      <c r="F18" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="D19" s="3" t="str">
+      <c r="D19" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F19" s="3" t="str">
+      <c r="F19" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4493,35 +4499,35 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>2</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="3">
+      <c r="A2" s="1">
         <v>1.0</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>47</v>
+      <c r="B2" s="12" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="3">
+      <c r="A3" s="1">
         <v>2.0</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>55</v>
+      <c r="B3" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="3">
+      <c r="A4" s="1">
         <v>3.0</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>57</v>
+      <c r="B4" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
fix: japanese lang string sheet name.
</commit_message>
<xml_diff>
--- a/data/spreadsheet.xlsx
+++ b/data/spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="talking" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="話すこと" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="events" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="rankings" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="users" sheetId="4" r:id="rId7"/>
@@ -16,12 +16,21 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
   <si>
+    <t>スプレットシートマスター</t>
+  </si>
+  <si>
+    <t>目的</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
     <t>rank</t>
   </si>
   <si>
+    <t>name</t>
+  </si>
+  <si>
     <t>event_id</t>
   </si>
   <si>
@@ -29,12 +38,6 @@
   </si>
   <si>
     <t>user_id</t>
-  </si>
-  <si>
-    <t>スプレットシートマスター</t>
-  </si>
-  <si>
-    <t>name</t>
   </si>
   <si>
     <t>user_name</t>
@@ -48,9 +51,6 @@
   <si>
     <t>happy
 new year</t>
-  </si>
-  <si>
-    <t>目的</t>
   </si>
   <si>
     <t>スプレットシートで管理しているものを全部Gitで管理しようというもの</t>
@@ -273,18 +273,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
@@ -298,6 +298,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -598,37 +601,37 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>11</v>
+      <c r="A2" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -661,14 +664,14 @@
       <c r="Y3" s="5"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="7"/>
     </row>
     <row r="5">
       <c r="A5" s="7"/>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -703,270 +706,270 @@
     </row>
     <row r="7">
       <c r="B7" s="7"/>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8">
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9">
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="C10" s="7"/>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11">
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12">
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13">
       <c r="C13" s="7"/>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E13" s="7"/>
     </row>
     <row r="14">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="7"/>
     </row>
     <row r="15">
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16">
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17">
       <c r="D17" s="7"/>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18">
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="7"/>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="20">
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E22" s="10"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E23" s="7"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E24" s="7"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="C25" s="7"/>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="C26" s="7"/>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D27" s="7"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="C29" s="7"/>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="D30" s="7"/>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="C32" s="7"/>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D33" s="7"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D34" s="7"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="C36" s="7"/>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="D37" s="7"/>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E38" s="7"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E39" s="7"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="C41" s="7"/>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="D42" s="7"/>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="C44" s="7"/>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C45" s="7"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D47" s="7"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>57</v>
       </c>
       <c r="E48" s="7"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C50" s="7"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="3" t="s">
         <v>60</v>
       </c>
       <c r="D51" s="7"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="3" t="s">
         <v>61</v>
       </c>
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="3" t="s">
         <v>62</v>
       </c>
       <c r="D53" s="7"/>
@@ -974,28 +977,31 @@
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="D54" s="7"/>
-      <c r="E54" s="7" t="s">
+      <c r="E54" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
+      <c r="A57" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="D57" s="7"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B58" s="11"/>
+      <c r="A58" s="11"/>
+      <c r="B58" s="12" t="s">
+        <v>55</v>
+      </c>
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
       <c r="E58" s="11"/>
@@ -1021,46 +1027,50 @@
       <c r="Y58" s="11"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="B59" s="7" t="s">
-        <v>55</v>
+      <c r="B59" s="7"/>
+      <c r="C59" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="C60" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="B60" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C60" s="7"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="B61" s="7" t="s">
-        <v>57</v>
+      <c r="B61" s="7"/>
+      <c r="C61" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="C62" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="63" ht="15.75" customHeight="1"/>
+      <c r="B62" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" s="7"/>
+    </row>
+    <row r="63" ht="15.75" customHeight="1">
+      <c r="C63" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="B64" s="12" t="s">
-        <v>59</v>
+      <c r="B64" s="13" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="C65" s="7" t="s">
-        <v>60</v>
+      <c r="C65" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="B67" s="7" t="s">
-        <v>61</v>
-      </c>
+      <c r="B67" s="7"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="C68" s="7" t="s">
-        <v>62</v>
-      </c>
+      <c r="C68" s="7"/>
     </row>
     <row r="69" ht="15.75" customHeight="1"/>
     <row r="70" ht="15.75" customHeight="1"/>
@@ -2013,27 +2023,27 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1">
+      <c r="A2" s="4">
         <v>1.0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1">
+      <c r="A3" s="4">
         <v>2.0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1"/>
@@ -3052,39 +3062,39 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1">
+      <c r="A2" s="4">
         <v>1.0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>1.0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>1.0</v>
       </c>
-      <c r="D2" s="1" t="str">
+      <c r="D2" s="4" t="str">
         <f t="array" ref="D2">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3100,10 +3110,10 @@
 )</f>
         <v>christmas</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="4">
         <v>1.0</v>
       </c>
-      <c r="F2" s="1" t="str">
+      <c r="F2" s="4" t="str">
         <f t="array" ref="F2">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3121,10 +3131,10 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>2.0</v>
       </c>
-      <c r="D3" s="1" t="str">
+      <c r="D3" s="4" t="str">
         <f t="array" ref="D3">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3141,10 +3151,10 @@
         <v>happy
 new year</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="4">
         <v>3.0</v>
       </c>
-      <c r="F3" s="1" t="str">
+      <c r="F3" s="4" t="str">
         <f t="array" ref="F3">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3162,7 +3172,7 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="D4" s="1" t="str">
+      <c r="D4" s="4" t="str">
         <f t="array" ref="D4">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3178,10 +3188,10 @@
 )</f>
         <v/>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <v>2.0</v>
       </c>
-      <c r="F4" s="1" t="str">
+      <c r="F4" s="4" t="str">
         <f t="array" ref="F4">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3199,7 +3209,7 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="D5" s="1" t="str">
+      <c r="D5" s="4" t="str">
         <f t="array" ref="D5">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3215,7 +3225,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F5" s="1" t="str">
+      <c r="F5" s="4" t="str">
         <f t="array" ref="F5">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3233,7 +3243,7 @@
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="D6" s="1" t="str">
+      <c r="D6" s="4" t="str">
         <f t="array" ref="D6">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3249,7 +3259,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F6" s="1" t="str">
+      <c r="F6" s="4" t="str">
         <f t="array" ref="F6">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3267,7 +3277,7 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="D7" s="1" t="str">
+      <c r="D7" s="4" t="str">
         <f t="array" ref="D7">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3283,7 +3293,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F7" s="1" t="str">
+      <c r="F7" s="4" t="str">
         <f t="array" ref="F7">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3301,7 +3311,7 @@
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="D8" s="1" t="str">
+      <c r="D8" s="4" t="str">
         <f t="array" ref="D8">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3317,7 +3327,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F8" s="1" t="str">
+      <c r="F8" s="4" t="str">
         <f t="array" ref="F8">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3335,7 +3345,7 @@
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="D9" s="1" t="str">
+      <c r="D9" s="4" t="str">
         <f t="array" ref="D9">IFERROR(
   INDEX(
     INDIRECT("'events'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", events!$1:$1, 0), 4), 1, "")),
@@ -3351,7 +3361,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F9" s="1" t="str">
+      <c r="F9" s="4" t="str">
         <f t="array" ref="F9">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3369,7 +3379,7 @@
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="F10" s="1" t="str">
+      <c r="F10" s="4" t="str">
         <f t="array" ref="F10">IFERROR(
   INDEX(
     INDIRECT("'users'" &amp; "!" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "") &amp; ":" &amp; SUBSTITUTE(ADDRESS(1, MATCH("name", users!$1:$1, 0), 4), 1, "")),
@@ -3387,19 +3397,19 @@
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="C11" s="1">
+      <c r="C11" s="4">
         <v>1.0</v>
       </c>
-      <c r="D11" s="1" t="str">
+      <c r="D11" s="4" t="str">
         <f t="shared" ref="D11:D19" si="1">GetCellFilterByColumnValue(
   "events!1:1!id," &amp; GetCellByColumnName("1:1," &amp; ROW(11:11) &amp; ",event_id") &amp;",name"
 )</f>
         <v>christmas</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="4">
         <v>1.0</v>
       </c>
-      <c r="F11" s="1" t="str">
+      <c r="F11" s="4" t="str">
         <f t="shared" ref="F11:F19" si="2">GetCellFilterByColumnValue(
   "users!1:1!id," &amp; GetCellByColumnName("1:1," &amp; ROW(11:11) &amp; ",user_id") &amp;",name"
 )</f>
@@ -3407,94 +3417,94 @@
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="C12" s="1">
+      <c r="C12" s="4">
         <v>2.0</v>
       </c>
-      <c r="D12" s="1" t="str">
+      <c r="D12" s="4" t="str">
         <f t="shared" si="1"/>
         <v>happy
 new year</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="4">
         <v>2.0</v>
       </c>
-      <c r="F12" s="1" t="str">
+      <c r="F12" s="4" t="str">
         <f t="shared" si="2"/>
         <v>jiro</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="D13" s="1" t="str">
+      <c r="D13" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="4">
         <v>3.0</v>
       </c>
-      <c r="F13" s="1" t="str">
+      <c r="F13" s="4" t="str">
         <f t="shared" si="2"/>
         <v>saburo</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="B14" s="1">
+      <c r="B14" s="4">
         <v>5.0</v>
       </c>
-      <c r="D14" s="1" t="str">
+      <c r="D14" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F14" s="1" t="str">
+      <c r="F14" s="4" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="D15" s="1" t="str">
+      <c r="D15" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F15" s="1" t="str">
+      <c r="F15" s="4" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="D16" s="1" t="str">
+      <c r="D16" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F16" s="1" t="str">
+      <c r="F16" s="4" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="D17" s="1" t="str">
+      <c r="D17" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F17" s="1" t="str">
+      <c r="F17" s="4" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="D18" s="1" t="str">
+      <c r="D18" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F18" s="1" t="str">
+      <c r="F18" s="4" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="D19" s="1" t="str">
+      <c r="D19" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F19" s="1" t="str">
+      <c r="F19" s="4" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -4499,34 +4509,34 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1">
+      <c r="A2" s="4">
         <v>1.0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1">
+      <c r="A3" s="4">
         <v>2.0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1">
+      <c r="A4" s="4">
         <v>3.0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>